<commit_message>
Armazenamento dos valores como número
</commit_message>
<xml_diff>
--- a/web-scraping/atualizar-indicadores-fiis/atualizar-indicadores-fiis.xlsx
+++ b/web-scraping/atualizar-indicadores-fiis/atualizar-indicadores-fiis.xlsx
@@ -801,20 +801,14 @@
           <t>BTHF11</t>
         </is>
       </c>
-      <c r="C3" s="11" t="inlineStr">
-        <is>
-          <t>8,32</t>
-        </is>
-      </c>
-      <c r="D3" s="11" t="inlineStr">
-        <is>
-          <t>9,89</t>
-        </is>
-      </c>
-      <c r="E3" s="9" t="inlineStr">
-        <is>
-          <t>6,80%</t>
-        </is>
+      <c r="C3" s="11" t="n">
+        <v>8.539999999999999</v>
+      </c>
+      <c r="D3" s="11" t="n">
+        <v>9.890000000000001</v>
+      </c>
+      <c r="E3" s="9" t="n">
+        <v>0.07730000000000001</v>
       </c>
     </row>
     <row r="4" ht="13.2" customHeight="1">
@@ -823,20 +817,14 @@
           <t>BTLG11</t>
         </is>
       </c>
-      <c r="C4" s="11" t="inlineStr">
-        <is>
-          <t>100,25</t>
-        </is>
-      </c>
-      <c r="D4" s="11" t="inlineStr">
-        <is>
-          <t>104,00</t>
-        </is>
-      </c>
-      <c r="E4" s="9" t="inlineStr">
-        <is>
-          <t>9,35%</t>
-        </is>
+      <c r="C4" s="11" t="n">
+        <v>100.43</v>
+      </c>
+      <c r="D4" s="11" t="n">
+        <v>104</v>
+      </c>
+      <c r="E4" s="9" t="n">
+        <v>0.0934</v>
       </c>
     </row>
     <row r="5" ht="13.2" customHeight="1">
@@ -845,20 +833,14 @@
           <t>HGRU11</t>
         </is>
       </c>
-      <c r="C5" s="11" t="inlineStr">
-        <is>
-          <t>124,45</t>
-        </is>
-      </c>
-      <c r="D5" s="11" t="inlineStr">
-        <is>
-          <t>125,56</t>
-        </is>
-      </c>
-      <c r="E5" s="9" t="inlineStr">
-        <is>
-          <t>9,58%</t>
-        </is>
+      <c r="C5" s="11" t="n">
+        <v>124.6</v>
+      </c>
+      <c r="D5" s="11" t="n">
+        <v>125.56</v>
+      </c>
+      <c r="E5" s="9" t="n">
+        <v>0.09669999999999999</v>
       </c>
     </row>
     <row r="6" ht="13.2" customHeight="1">
@@ -867,20 +849,14 @@
           <t>KNCR11</t>
         </is>
       </c>
-      <c r="C6" s="11" t="inlineStr">
-        <is>
-          <t>103,80</t>
-        </is>
-      </c>
-      <c r="D6" s="11" t="inlineStr">
-        <is>
-          <t>101,74</t>
-        </is>
-      </c>
-      <c r="E6" s="9" t="inlineStr">
-        <is>
-          <t>11,70%</t>
-        </is>
+      <c r="C6" s="11" t="n">
+        <v>102.35</v>
+      </c>
+      <c r="D6" s="11" t="n">
+        <v>101.74</v>
+      </c>
+      <c r="E6" s="9" t="n">
+        <v>0.121</v>
       </c>
     </row>
     <row r="7" ht="13.2" customHeight="1">
@@ -889,20 +865,14 @@
           <t>MXRF11</t>
         </is>
       </c>
-      <c r="C7" s="11" t="inlineStr">
-        <is>
-          <t>9,59</t>
-        </is>
-      </c>
-      <c r="D7" s="11" t="inlineStr">
-        <is>
-          <t>9,40</t>
-        </is>
-      </c>
-      <c r="E7" s="9" t="inlineStr">
-        <is>
-          <t>11,90%</t>
-        </is>
+      <c r="C7" s="11" t="n">
+        <v>9.25</v>
+      </c>
+      <c r="D7" s="11" t="n">
+        <v>9.4</v>
+      </c>
+      <c r="E7" s="9" t="n">
+        <v>0.1236</v>
       </c>
     </row>
     <row r="8" ht="13.2" customHeight="1">
@@ -911,20 +881,14 @@
           <t>TRXF11</t>
         </is>
       </c>
-      <c r="C8" s="11" t="inlineStr">
-        <is>
-          <t>102,20</t>
-        </is>
-      </c>
-      <c r="D8" s="11" t="inlineStr">
-        <is>
-          <t>101,72</t>
-        </is>
-      </c>
-      <c r="E8" s="9" t="inlineStr">
-        <is>
-          <t>12,54%</t>
-        </is>
+      <c r="C8" s="11" t="n">
+        <v>100.4</v>
+      </c>
+      <c r="D8" s="11" t="n">
+        <v>101.72</v>
+      </c>
+      <c r="E8" s="9" t="n">
+        <v>0.1279</v>
       </c>
     </row>
     <row r="9" ht="13.2" customHeight="1">
@@ -933,20 +897,14 @@
           <t>VGHF11</t>
         </is>
       </c>
-      <c r="C9" s="11" t="inlineStr">
-        <is>
-          <t>7,74</t>
-        </is>
-      </c>
-      <c r="D9" s="11" t="inlineStr">
-        <is>
-          <t>8,54</t>
-        </is>
-      </c>
-      <c r="E9" s="9" t="inlineStr">
-        <is>
-          <t>13,84%</t>
-        </is>
+      <c r="C9" s="11" t="n">
+        <v>7.42</v>
+      </c>
+      <c r="D9" s="11" t="n">
+        <v>8.539999999999999</v>
+      </c>
+      <c r="E9" s="9" t="n">
+        <v>0.144</v>
       </c>
     </row>
     <row r="10" ht="13.2" customHeight="1">
@@ -955,20 +913,14 @@
           <t>VISC11</t>
         </is>
       </c>
-      <c r="C10" s="11" t="inlineStr">
-        <is>
-          <t>104,15</t>
-        </is>
-      </c>
-      <c r="D10" s="11" t="inlineStr">
-        <is>
-          <t>124,34</t>
-        </is>
-      </c>
-      <c r="E10" s="9" t="inlineStr">
-        <is>
-          <t>9,54%</t>
-        </is>
+      <c r="C10" s="11" t="n">
+        <v>101.02</v>
+      </c>
+      <c r="D10" s="11" t="n">
+        <v>124.34</v>
+      </c>
+      <c r="E10" s="9" t="n">
+        <v>0.09619999999999999</v>
       </c>
     </row>
     <row r="11" ht="13.2" customHeight="1">
@@ -977,20 +929,14 @@
           <t>XPLG11</t>
         </is>
       </c>
-      <c r="C11" s="11" t="inlineStr">
-        <is>
-          <t>100,01</t>
-        </is>
-      </c>
-      <c r="D11" s="11" t="inlineStr">
-        <is>
-          <t>106,75</t>
-        </is>
-      </c>
-      <c r="E11" s="9" t="inlineStr">
-        <is>
-          <t>9,48%</t>
-        </is>
+      <c r="C11" s="11" t="n">
+        <v>97.2</v>
+      </c>
+      <c r="D11" s="11" t="n">
+        <v>106.75</v>
+      </c>
+      <c r="E11" s="9" t="n">
+        <v>0.09859999999999999</v>
       </c>
     </row>
     <row r="12" ht="13.2" customHeight="1">
@@ -999,20 +945,14 @@
           <t>XPML11</t>
         </is>
       </c>
-      <c r="C12" s="12" t="inlineStr">
-        <is>
-          <t>104,95</t>
-        </is>
-      </c>
-      <c r="D12" s="12" t="inlineStr">
-        <is>
-          <t>117,39</t>
-        </is>
-      </c>
-      <c r="E12" s="10" t="inlineStr">
-        <is>
-          <t>10,54%</t>
-        </is>
+      <c r="C12" s="12" t="n">
+        <v>103.05</v>
+      </c>
+      <c r="D12" s="12" t="n">
+        <v>117.39</v>
+      </c>
+      <c r="E12" s="10" t="n">
+        <v>0.1072</v>
       </c>
     </row>
     <row r="13" ht="13.2" customHeight="1"/>

</xml_diff>